<commit_message>
got the evalaution results and finished the dissimiarity matrix graph tools, plus a results summary page
</commit_message>
<xml_diff>
--- a/documentation/writeUp/evaluationJobs.xlsx
+++ b/documentation/writeUp/evaluationJobs.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\projects\clusterColombia\climacolombia\documentation\writeUp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C9F03F1-E665-4CFC-8C26-D4B8B102F614}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7D0C9CA5-3659-4567-9D76-6EF27F1EA926}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{DC76DEBC-A1F9-45F2-A205-10806F0ABE5F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
+  <pivotCaches>
+    <pivotCache cacheId="10" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="70">
   <si>
     <t>KM</t>
   </si>
@@ -57,9 +61,6 @@
     <t>method</t>
   </si>
   <si>
-    <t>t</t>
-  </si>
-  <si>
     <t>$</t>
   </si>
   <si>
@@ -85,13 +86,169 @@
   </si>
   <si>
     <t>ideamci</t>
+  </si>
+  <si>
+    <t>r4.xlarge</t>
+  </si>
+  <si>
+    <t>per Hour</t>
+  </si>
+  <si>
+    <t>per min</t>
+  </si>
+  <si>
+    <t>per sec</t>
+  </si>
+  <si>
+    <t>analysis</t>
+  </si>
+  <si>
+    <t>dashboard</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>check the strategies look good</t>
+  </si>
+  <si>
+    <t>10 instances</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_11_53_39/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_11_53_30/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_11_46_08/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_12_58_07/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_14_20_42/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_14_20_00/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_14_18_36/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_14_06_53/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_14_06_45/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_14_21_03/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_14_20_56/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_26_14_53_14/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_26_14_14_21/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_11_20_24/</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_11_21_05/</t>
+  </si>
+  <si>
+    <t>total mins</t>
+  </si>
+  <si>
+    <t>total secs</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>KM6TRh</t>
+  </si>
+  <si>
+    <t>KM11TRh</t>
+  </si>
+  <si>
+    <t>BKM11TRh</t>
+  </si>
+  <si>
+    <t>KM6TrRh</t>
+  </si>
+  <si>
+    <t>KM11TrRh</t>
+  </si>
+  <si>
+    <t>KM11TRhWs</t>
+  </si>
+  <si>
+    <t>KM11TTrRhWs</t>
+  </si>
+  <si>
+    <t>KM6TRhWs</t>
+  </si>
+  <si>
+    <t>KM6TTrRhWs</t>
+  </si>
+  <si>
+    <t>BKM6TRh</t>
+  </si>
+  <si>
+    <t>BKM6TrRh</t>
+  </si>
+  <si>
+    <t>BKM11TrRh</t>
+  </si>
+  <si>
+    <t>BKM11TRhWs</t>
+  </si>
+  <si>
+    <t>BKM11TTrRhWs</t>
+  </si>
+  <si>
+    <t>BKM6TRhWs</t>
+  </si>
+  <si>
+    <t>BKM6TTrRhWs</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dunn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wssse</t>
+  </si>
+  <si>
+    <t>sd utci</t>
+  </si>
+  <si>
+    <t>ideamci sd</t>
+  </si>
+  <si>
+    <t>http://lacunae.io/geovis2018_10_27_15_05_38/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,16 +262,55 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -159,11 +355,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -171,8 +420,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" textRotation="90"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -186,6 +473,464 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Admin" refreshedDate="43400.650348263887" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="16" xr:uid="{ABBE4D84-670B-4941-AE58-4C1CB524E737}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="E2:Q18" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="13">
+    <cacheField name="name" numFmtId="0">
+      <sharedItems count="16">
+        <s v="KM6TRh"/>
+        <s v="KM6TrRh"/>
+        <s v="KM6TRhWs"/>
+        <s v="KM6TTrRhWs"/>
+        <s v="BKM6TRh"/>
+        <s v="BKM6TrRh"/>
+        <s v="BKM6TRhWs"/>
+        <s v="BKM6TTrRhWs"/>
+        <s v="KM11TRh"/>
+        <s v="KM11TrRh"/>
+        <s v="KM11TRhWs"/>
+        <s v="KM11TTrRhWs"/>
+        <s v="BKM11TRh"/>
+        <s v="BKM11TrRh"/>
+        <s v="BKM11TRhWs"/>
+        <s v="BKM11TTrRhWs"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="total mins" numFmtId="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="27.466666666666665" maxValue="70.7"/>
+    </cacheField>
+    <cacheField name="total secs" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1648" maxValue="4242"/>
+    </cacheField>
+    <cacheField name="$" numFmtId="172">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.3067111111111111" maxValue="0.78948333333333343"/>
+    </cacheField>
+    <cacheField name="sil" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.77" maxValue="0.99"/>
+    </cacheField>
+    <cacheField name="dunn" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.56" maxValue="8.4600000000000009"/>
+    </cacheField>
+    <cacheField name="wssse" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.68" maxValue="54.25"/>
+    </cacheField>
+    <cacheField name="mean" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.49" maxValue="1.93"/>
+    </cacheField>
+    <cacheField name="sd" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.0699999999999998" maxValue="5.29"/>
+    </cacheField>
+    <cacheField name="rmse" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.17" maxValue="5.63"/>
+    </cacheField>
+    <cacheField name="mean2" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-0.67" maxValue="-0.09"/>
+    </cacheField>
+    <cacheField name="sd2" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.25" maxValue="3.18"/>
+    </cacheField>
+    <cacheField name="rmse2" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.27" maxValue="3.25"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="16">
+  <r>
+    <x v="0"/>
+    <n v="28.6"/>
+    <n v="1716"/>
+    <n v="0.31936666666666669"/>
+    <n v="0.97"/>
+    <n v="3.53"/>
+    <n v="7.6"/>
+    <n v="1.24"/>
+    <n v="3.12"/>
+    <n v="3.35"/>
+    <n v="-0.14000000000000001"/>
+    <n v="1.36"/>
+    <n v="1.36"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="33.18333333333333"/>
+    <n v="1991"/>
+    <n v="0.37054722222222219"/>
+    <n v="0.97"/>
+    <n v="4"/>
+    <n v="1.98"/>
+    <n v="1.91"/>
+    <n v="5.28"/>
+    <n v="5.61"/>
+    <n v="-0.64"/>
+    <n v="3.16"/>
+    <n v="3.23"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="44.733333333333334"/>
+    <n v="2684"/>
+    <n v="0.49952222222222226"/>
+    <n v="0.87"/>
+    <n v="2.92"/>
+    <n v="34.450000000000003"/>
+    <n v="0.94"/>
+    <n v="2.85"/>
+    <n v="3"/>
+    <n v="-0.26"/>
+    <n v="1.45"/>
+    <n v="1.47"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="45.43333333333333"/>
+    <n v="2726"/>
+    <n v="0.50733888888888889"/>
+    <n v="0.77"/>
+    <n v="2.85"/>
+    <n v="51.21"/>
+    <n v="0.98"/>
+    <n v="2.82"/>
+    <n v="2.99"/>
+    <n v="-0.24"/>
+    <n v="1.44"/>
+    <n v="1.46"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="27.466666666666665"/>
+    <n v="1648"/>
+    <n v="0.3067111111111111"/>
+    <n v="0.97"/>
+    <n v="3.8"/>
+    <n v="7.63"/>
+    <n v="1.41"/>
+    <n v="3.04"/>
+    <n v="3.35"/>
+    <n v="-0.24"/>
+    <n v="1.34"/>
+    <n v="1.36"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="43.366666666666667"/>
+    <n v="2602"/>
+    <n v="0.48426111111111114"/>
+    <n v="0.93"/>
+    <n v="2.65"/>
+    <n v="2.39"/>
+    <n v="1.93"/>
+    <n v="5.29"/>
+    <n v="5.63"/>
+    <n v="-0.67"/>
+    <n v="3.18"/>
+    <n v="3.25"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="45.666666666666664"/>
+    <n v="2740"/>
+    <n v="0.50994444444444442"/>
+    <n v="0.84"/>
+    <n v="2.78"/>
+    <n v="36.04"/>
+    <n v="0.84"/>
+    <n v="2.76"/>
+    <n v="2.88"/>
+    <n v="-0.26"/>
+    <n v="1.34"/>
+    <n v="1.37"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="45.31666666666667"/>
+    <n v="2719"/>
+    <n v="0.50603611111111113"/>
+    <n v="0.77"/>
+    <n v="2.56"/>
+    <n v="54.25"/>
+    <n v="1.06"/>
+    <n v="3.17"/>
+    <n v="3.35"/>
+    <n v="-0.33"/>
+    <n v="1.71"/>
+    <n v="1.74"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="43.716666666666669"/>
+    <n v="2623"/>
+    <n v="0.48816944444444449"/>
+    <n v="0.99"/>
+    <n v="5.84"/>
+    <n v="2.5099999999999998"/>
+    <n v="1.28"/>
+    <n v="2.92"/>
+    <n v="3.18"/>
+    <n v="-0.16"/>
+    <n v="1.26"/>
+    <n v="1.27"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="44.333333333333336"/>
+    <n v="2660"/>
+    <n v="0.49505555555555558"/>
+    <n v="0.99"/>
+    <n v="8.4600000000000009"/>
+    <n v="0.68"/>
+    <n v="1.93"/>
+    <n v="5.28"/>
+    <n v="5.62"/>
+    <n v="-0.65"/>
+    <n v="3.17"/>
+    <n v="3.23"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="70.7"/>
+    <n v="4242"/>
+    <n v="0.78948333333333343"/>
+    <n v="0.93"/>
+    <n v="4.4000000000000004"/>
+    <n v="19.010000000000002"/>
+    <n v="0.49"/>
+    <n v="2.35"/>
+    <n v="2.4"/>
+    <n v="-0.09"/>
+    <n v="1.29"/>
+    <n v="1.29"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="67.683333333333337"/>
+    <n v="4061"/>
+    <n v="0.75579722222222223"/>
+    <n v="0.88"/>
+    <n v="4.13"/>
+    <n v="34.83"/>
+    <n v="0.6"/>
+    <n v="2.7"/>
+    <n v="2.77"/>
+    <n v="-0.11"/>
+    <n v="1.39"/>
+    <n v="1.39"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="43.733333333333334"/>
+    <n v="2624"/>
+    <n v="0.48835555555555554"/>
+    <n v="0.99"/>
+    <n v="4.1399999999999997"/>
+    <n v="2.8"/>
+    <n v="1.33"/>
+    <n v="2.88"/>
+    <n v="3.17"/>
+    <n v="-0.2"/>
+    <n v="1.29"/>
+    <n v="1.3"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="65.3"/>
+    <n v="3918"/>
+    <n v="0.72918333333333329"/>
+    <n v="0.98"/>
+    <n v="5.04"/>
+    <n v="0.83"/>
+    <n v="1.93"/>
+    <n v="5.27"/>
+    <n v="5.61"/>
+    <n v="-0.66"/>
+    <n v="3.18"/>
+    <n v="3.24"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="68.8"/>
+    <n v="4128"/>
+    <n v="0.76826666666666665"/>
+    <n v="0.9"/>
+    <n v="2.93"/>
+    <n v="21.43"/>
+    <n v="0.65"/>
+    <n v="2.0699999999999998"/>
+    <n v="2.17"/>
+    <n v="-0.18"/>
+    <n v="1.25"/>
+    <n v="1.27"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <n v="41.666666666666664"/>
+    <n v="2500"/>
+    <n v="0.46527777777777773"/>
+    <n v="0.82"/>
+    <n v="2.92"/>
+    <n v="38.07"/>
+    <n v="0.71"/>
+    <n v="2.76"/>
+    <n v="2.85"/>
+    <n v="-0.23"/>
+    <n v="1.58"/>
+    <n v="1.6"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8220A296-A18E-454C-BAA6-84CDAD8FFF81}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:F20" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="13">
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="17">
+        <item x="12"/>
+        <item x="14"/>
+        <item x="13"/>
+        <item x="15"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="11"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField numFmtId="2" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="172" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="17">
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </colItems>
+  <dataFields count="5">
+    <dataField name=" dunn" fld="5" baseField="0" baseItem="0"/>
+    <dataField name=" sil" fld="4" baseField="0" baseItem="0"/>
+    <dataField name=" wssse" fld="6" baseField="0" baseItem="0"/>
+    <dataField name="sd utci" fld="8" baseField="0" baseItem="0"/>
+    <dataField name="ideamci sd" fld="11" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -484,24 +1229,442 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC85AE9-E338-486B-9FD4-D48A83E178DE}">
-  <dimension ref="A1:O28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D958AE5-8B60-4C50-BFC1-A0CF9128626B}">
+  <dimension ref="A3:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="8">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.99</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0.68</v>
+      </c>
+      <c r="E4" s="8">
+        <v>5.28</v>
+      </c>
+      <c r="F4" s="8">
+        <v>3.17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="8">
+        <v>5.84</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.99</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2.92</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5.04</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.98</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.83</v>
+      </c>
+      <c r="E6" s="8">
+        <v>5.27</v>
+      </c>
+      <c r="F6" s="8">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.93</v>
+      </c>
+      <c r="D7" s="8">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2.35</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="8">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.99</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2.88</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="8">
+        <v>4.13</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.88</v>
+      </c>
+      <c r="D9" s="8">
+        <v>34.83</v>
+      </c>
+      <c r="E9" s="8">
+        <v>2.7</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="8">
+        <v>4</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1.98</v>
+      </c>
+      <c r="E10" s="8">
+        <v>5.28</v>
+      </c>
+      <c r="F10" s="8">
+        <v>3.16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="8">
+        <v>3.8</v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="D11" s="8">
+        <v>7.63</v>
+      </c>
+      <c r="E11" s="8">
+        <v>3.04</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="8">
+        <v>3.53</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="D12" s="8">
+        <v>7.6</v>
+      </c>
+      <c r="E12" s="8">
+        <v>3.12</v>
+      </c>
+      <c r="F12" s="8">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="8">
+        <v>2.93</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="D13" s="8">
+        <v>21.43</v>
+      </c>
+      <c r="E13" s="8">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2.92</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="D14" s="8">
+        <v>34.450000000000003</v>
+      </c>
+      <c r="E14" s="8">
+        <v>2.85</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="8">
+        <v>2.92</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.82</v>
+      </c>
+      <c r="D15" s="8">
+        <v>38.07</v>
+      </c>
+      <c r="E15" s="8">
+        <v>2.76</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="8">
+        <v>2.85</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.77</v>
+      </c>
+      <c r="D16" s="8">
+        <v>51.21</v>
+      </c>
+      <c r="E16" s="8">
+        <v>2.82</v>
+      </c>
+      <c r="F16" s="8">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="8">
+        <v>2.78</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.84</v>
+      </c>
+      <c r="D17" s="8">
+        <v>36.04</v>
+      </c>
+      <c r="E17" s="8">
+        <v>2.76</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="8">
+        <v>2.65</v>
+      </c>
+      <c r="C18" s="8">
+        <v>0.93</v>
+      </c>
+      <c r="D18" s="8">
+        <v>2.39</v>
+      </c>
+      <c r="E18" s="8">
+        <v>5.29</v>
+      </c>
+      <c r="F18" s="8">
+        <v>3.18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="8">
+        <v>2.56</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0.77</v>
+      </c>
+      <c r="D19" s="8">
+        <v>54.25</v>
+      </c>
+      <c r="E19" s="8">
+        <v>3.17</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="8">
+        <v>62.95</v>
+      </c>
+      <c r="C20" s="8">
+        <v>14.57</v>
+      </c>
+      <c r="D20" s="8">
+        <v>315.70999999999998</v>
+      </c>
+      <c r="E20" s="8">
+        <v>54.560000000000009</v>
+      </c>
+      <c r="F20" s="8">
+        <v>29.390000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AC85AE9-E338-486B-9FD4-D48A83E178DE}">
+  <dimension ref="A1:W28"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="7" max="12" width="5.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="5.7109375" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" customWidth="1"/>
+    <col min="20" max="20" width="44" customWidth="1"/>
+    <col min="21" max="21" width="22.140625" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="43.5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -511,41 +1674,56 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="L2" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="O2" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="O2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="U2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" s="5">
+        <v>0.67</v>
+      </c>
+      <c r="W2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -558,8 +1736,65 @@
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E3" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="12">
+        <f>G3/60</f>
+        <v>28.6</v>
+      </c>
+      <c r="G3" s="24">
+        <v>1716</v>
+      </c>
+      <c r="H3" s="15">
+        <f>F3*$V$3</f>
+        <v>0.31936666666666669</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0.97</v>
+      </c>
+      <c r="J3" s="11">
+        <v>3.53</v>
+      </c>
+      <c r="K3" s="11">
+        <v>7.6</v>
+      </c>
+      <c r="L3" s="16">
+        <v>1.24</v>
+      </c>
+      <c r="M3" s="16">
+        <v>3.12</v>
+      </c>
+      <c r="N3" s="16">
+        <v>3.35</v>
+      </c>
+      <c r="O3" s="11">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="P3" s="11">
+        <v>1.36</v>
+      </c>
+      <c r="Q3" s="11">
+        <v>1.36</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3">
+        <f>V2/60</f>
+        <v>1.1166666666666667E-2</v>
+      </c>
+      <c r="W3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -569,8 +1804,65 @@
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="12">
+        <f>G4/60</f>
+        <v>33.18333333333333</v>
+      </c>
+      <c r="G4" s="24">
+        <v>1991</v>
+      </c>
+      <c r="H4" s="15">
+        <f>F4*$V$3</f>
+        <v>0.37054722222222219</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.97</v>
+      </c>
+      <c r="J4" s="11">
+        <v>4</v>
+      </c>
+      <c r="K4" s="11">
+        <v>1.98</v>
+      </c>
+      <c r="L4" s="16">
+        <v>1.91</v>
+      </c>
+      <c r="M4" s="16">
+        <v>5.28</v>
+      </c>
+      <c r="N4" s="16">
+        <v>5.61</v>
+      </c>
+      <c r="O4" s="11">
+        <v>-0.64</v>
+      </c>
+      <c r="P4" s="11">
+        <v>3.16</v>
+      </c>
+      <c r="Q4" s="11">
+        <v>3.23</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="V4">
+        <f>V3/60</f>
+        <v>1.8611111111111112E-4</v>
+      </c>
+      <c r="W4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -580,8 +1872,61 @@
       <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E5" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="12">
+        <f t="shared" ref="F5:F18" si="0">G5/60</f>
+        <v>44.733333333333334</v>
+      </c>
+      <c r="G5" s="24">
+        <v>2684</v>
+      </c>
+      <c r="H5" s="15">
+        <f t="shared" ref="H5:H18" si="1">F5*$V$3</f>
+        <v>0.49952222222222226</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0.87</v>
+      </c>
+      <c r="J5" s="11">
+        <v>2.92</v>
+      </c>
+      <c r="K5" s="11">
+        <v>34.450000000000003</v>
+      </c>
+      <c r="L5" s="16">
+        <v>0.94</v>
+      </c>
+      <c r="M5" s="16">
+        <v>2.85</v>
+      </c>
+      <c r="N5" s="16">
+        <v>3</v>
+      </c>
+      <c r="O5" s="11">
+        <v>-0.26</v>
+      </c>
+      <c r="P5" s="11">
+        <v>1.45</v>
+      </c>
+      <c r="Q5" s="11">
+        <v>1.47</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="V5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -591,110 +1936,619 @@
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="0"/>
+        <v>45.43333333333333</v>
+      </c>
+      <c r="G6" s="24">
+        <v>2726</v>
+      </c>
+      <c r="H6" s="15">
+        <f t="shared" si="1"/>
+        <v>0.50733888888888889</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0.77</v>
+      </c>
+      <c r="J6" s="11">
+        <v>2.85</v>
+      </c>
+      <c r="K6" s="11">
+        <v>51.21</v>
+      </c>
+      <c r="L6" s="16">
+        <v>0.98</v>
+      </c>
+      <c r="M6" s="16">
+        <v>2.82</v>
+      </c>
+      <c r="N6" s="16">
+        <v>2.99</v>
+      </c>
+      <c r="O6" s="11">
+        <v>-0.24</v>
+      </c>
+      <c r="P6" s="11">
+        <v>1.44</v>
+      </c>
+      <c r="Q6" s="11">
+        <v>1.46</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="V6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
       <c r="C7">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E7" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="12">
+        <f>G7/60</f>
+        <v>27.466666666666665</v>
+      </c>
+      <c r="G7" s="24">
+        <v>1648</v>
+      </c>
+      <c r="H7" s="15">
+        <f>F7*$V$3</f>
+        <v>0.3067111111111111</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.97</v>
+      </c>
+      <c r="J7" s="11">
+        <v>3.8</v>
+      </c>
+      <c r="K7" s="11">
+        <v>7.63</v>
+      </c>
+      <c r="L7" s="16">
+        <v>1.41</v>
+      </c>
+      <c r="M7" s="16">
+        <v>3.04</v>
+      </c>
+      <c r="N7" s="16">
+        <v>3.35</v>
+      </c>
+      <c r="O7" s="11">
+        <v>-0.24</v>
+      </c>
+      <c r="P7" s="11">
+        <v>1.34</v>
+      </c>
+      <c r="Q7" s="11">
+        <v>1.36</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="C8">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="12">
+        <f>G8/60</f>
+        <v>43.366666666666667</v>
+      </c>
+      <c r="G8" s="24">
+        <v>2602</v>
+      </c>
+      <c r="H8" s="15">
+        <f>F8*$V$3</f>
+        <v>0.48426111111111114</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0.93</v>
+      </c>
+      <c r="J8" s="11">
+        <v>2.65</v>
+      </c>
+      <c r="K8" s="11">
+        <v>2.39</v>
+      </c>
+      <c r="L8" s="16">
+        <v>1.93</v>
+      </c>
+      <c r="M8" s="16">
+        <v>5.29</v>
+      </c>
+      <c r="N8" s="16">
+        <v>5.63</v>
+      </c>
+      <c r="O8" s="11">
+        <v>-0.67</v>
+      </c>
+      <c r="P8" s="11">
+        <v>3.18</v>
+      </c>
+      <c r="Q8" s="11">
+        <v>3.25</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="C9">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E9" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="12">
+        <f>G9/60</f>
+        <v>45.666666666666664</v>
+      </c>
+      <c r="G9" s="25">
+        <v>2740</v>
+      </c>
+      <c r="H9" s="15">
+        <f>F9*$V$3</f>
+        <v>0.50994444444444442</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0.84</v>
+      </c>
+      <c r="J9" s="11">
+        <v>2.78</v>
+      </c>
+      <c r="K9" s="11">
+        <v>36.04</v>
+      </c>
+      <c r="L9" s="16">
+        <v>0.84</v>
+      </c>
+      <c r="M9" s="16">
+        <v>2.76</v>
+      </c>
+      <c r="N9" s="16">
+        <v>2.88</v>
+      </c>
+      <c r="O9" s="11">
+        <v>-0.26</v>
+      </c>
+      <c r="P9" s="11">
+        <v>1.34</v>
+      </c>
+      <c r="Q9" s="11">
+        <v>1.37</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="C10">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E10" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="12">
+        <f>G10/60</f>
+        <v>45.31666666666667</v>
+      </c>
+      <c r="G10" s="24">
+        <v>2719</v>
+      </c>
+      <c r="H10" s="15">
+        <f>F10*$V$3</f>
+        <v>0.50603611111111113</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0.77</v>
+      </c>
+      <c r="J10" s="11">
+        <v>2.56</v>
+      </c>
+      <c r="K10" s="11">
+        <v>54.25</v>
+      </c>
+      <c r="L10" s="16">
+        <v>1.06</v>
+      </c>
+      <c r="M10" s="16">
+        <v>3.17</v>
+      </c>
+      <c r="N10" s="16">
+        <v>3.35</v>
+      </c>
+      <c r="O10" s="11">
+        <v>-0.33</v>
+      </c>
+      <c r="P10" s="11">
+        <v>1.71</v>
+      </c>
+      <c r="Q10" s="11">
+        <v>1.74</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="12">
+        <f>G11/60</f>
+        <v>43.716666666666669</v>
+      </c>
+      <c r="G11" s="24">
+        <v>2623</v>
+      </c>
+      <c r="H11" s="15">
+        <f>F11*$V$3</f>
+        <v>0.48816944444444449</v>
+      </c>
+      <c r="I11" s="11">
+        <v>0.99</v>
+      </c>
+      <c r="J11" s="11">
+        <v>5.84</v>
+      </c>
+      <c r="K11" s="11">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="L11" s="16">
+        <v>1.28</v>
+      </c>
+      <c r="M11" s="16">
+        <v>2.92</v>
+      </c>
+      <c r="N11" s="16">
+        <v>3.18</v>
+      </c>
+      <c r="O11" s="11">
+        <v>-0.16</v>
+      </c>
+      <c r="P11" s="11">
+        <v>1.26</v>
+      </c>
+      <c r="Q11" s="11">
+        <v>1.27</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="C12">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="12">
+        <f>G12/60</f>
+        <v>44.333333333333336</v>
+      </c>
+      <c r="G12" s="24">
+        <v>2660</v>
+      </c>
+      <c r="H12" s="15">
+        <f>F12*$V$3</f>
+        <v>0.49505555555555558</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0.99</v>
+      </c>
+      <c r="J12" s="11">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0.68</v>
+      </c>
+      <c r="L12" s="16">
+        <v>1.93</v>
+      </c>
+      <c r="M12" s="16">
+        <v>5.28</v>
+      </c>
+      <c r="N12" s="16">
+        <v>5.62</v>
+      </c>
+      <c r="O12" s="11">
+        <v>-0.65</v>
+      </c>
+      <c r="P12" s="11">
+        <v>3.17</v>
+      </c>
+      <c r="Q12" s="11">
+        <v>3.23</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="C13">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="12">
+        <f>G13/60</f>
+        <v>70.7</v>
+      </c>
+      <c r="G13" s="24">
+        <v>4242</v>
+      </c>
+      <c r="H13" s="15">
+        <f>F13*$V$3</f>
+        <v>0.78948333333333343</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0.93</v>
+      </c>
+      <c r="J13" s="11">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K13" s="11">
+        <v>19.010000000000002</v>
+      </c>
+      <c r="L13" s="16">
+        <v>0.49</v>
+      </c>
+      <c r="M13" s="16">
+        <v>2.35</v>
+      </c>
+      <c r="N13" s="16">
+        <v>2.4</v>
+      </c>
+      <c r="O13" s="11">
+        <v>-0.09</v>
+      </c>
+      <c r="P13" s="11">
+        <v>1.29</v>
+      </c>
+      <c r="Q13" s="11">
+        <v>1.29</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="T13" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="12">
+        <f>G14/60</f>
+        <v>67.683333333333337</v>
+      </c>
+      <c r="G14" s="24">
+        <v>4061</v>
+      </c>
+      <c r="H14" s="15">
+        <f>F14*$V$3</f>
+        <v>0.75579722222222223</v>
+      </c>
+      <c r="I14" s="11">
+        <v>0.88</v>
+      </c>
+      <c r="J14" s="11">
+        <v>4.13</v>
+      </c>
+      <c r="K14" s="11">
+        <v>34.83</v>
+      </c>
+      <c r="L14" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="M14" s="16">
+        <v>2.7</v>
+      </c>
+      <c r="N14" s="16">
+        <v>2.77</v>
+      </c>
+      <c r="O14" s="11">
+        <v>-0.11</v>
+      </c>
+      <c r="P14" s="11">
+        <v>1.39</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>1.39</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
       <c r="C15">
         <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E15" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="0"/>
+        <v>43.733333333333334</v>
+      </c>
+      <c r="G15" s="24">
+        <v>2624</v>
+      </c>
+      <c r="H15" s="15">
+        <f t="shared" si="1"/>
+        <v>0.48835555555555554</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0.99</v>
+      </c>
+      <c r="J15" s="11">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="K15" s="11">
+        <v>2.8</v>
+      </c>
+      <c r="L15" s="16">
+        <v>1.33</v>
+      </c>
+      <c r="M15" s="16">
+        <v>2.88</v>
+      </c>
+      <c r="N15" s="16">
+        <v>3.17</v>
+      </c>
+      <c r="O15" s="11">
+        <v>-0.2</v>
+      </c>
+      <c r="P15" s="11">
+        <v>1.29</v>
+      </c>
+      <c r="Q15" s="11">
+        <v>1.3</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -704,8 +2558,58 @@
       <c r="D16" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="0"/>
+        <v>65.3</v>
+      </c>
+      <c r="G16" s="24">
+        <v>3918</v>
+      </c>
+      <c r="H16" s="15">
+        <f t="shared" si="1"/>
+        <v>0.72918333333333329</v>
+      </c>
+      <c r="I16" s="11">
+        <v>0.98</v>
+      </c>
+      <c r="J16" s="11">
+        <v>5.04</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0.83</v>
+      </c>
+      <c r="L16" s="16">
+        <v>1.93</v>
+      </c>
+      <c r="M16" s="16">
+        <v>5.27</v>
+      </c>
+      <c r="N16" s="16">
+        <v>5.61</v>
+      </c>
+      <c r="O16" s="11">
+        <v>-0.66</v>
+      </c>
+      <c r="P16" s="11">
+        <v>3.18</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>3.24</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -715,8 +2619,58 @@
       <c r="D17" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E17" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="12">
+        <f t="shared" si="0"/>
+        <v>68.8</v>
+      </c>
+      <c r="G17" s="24">
+        <v>4128</v>
+      </c>
+      <c r="H17" s="15">
+        <f t="shared" si="1"/>
+        <v>0.76826666666666665</v>
+      </c>
+      <c r="I17" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="J17" s="11">
+        <v>2.93</v>
+      </c>
+      <c r="K17" s="11">
+        <v>21.43</v>
+      </c>
+      <c r="L17" s="16">
+        <v>0.65</v>
+      </c>
+      <c r="M17" s="16">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="N17" s="16">
+        <v>2.17</v>
+      </c>
+      <c r="O17" s="11">
+        <v>-0.18</v>
+      </c>
+      <c r="P17" s="11">
+        <v>1.25</v>
+      </c>
+      <c r="Q17" s="11">
+        <v>1.27</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -726,8 +2680,61 @@
       <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="0"/>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="G18" s="24">
+        <v>2500</v>
+      </c>
+      <c r="H18" s="15">
+        <f t="shared" si="1"/>
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="I18" s="11">
+        <v>0.82</v>
+      </c>
+      <c r="J18" s="11">
+        <v>2.92</v>
+      </c>
+      <c r="K18" s="11">
+        <v>38.07</v>
+      </c>
+      <c r="L18" s="16">
+        <v>0.71</v>
+      </c>
+      <c r="M18" s="16">
+        <v>2.76</v>
+      </c>
+      <c r="N18" s="16">
+        <v>2.85</v>
+      </c>
+      <c r="O18" s="11">
+        <v>-0.23</v>
+      </c>
+      <c r="P18" s="11">
+        <v>1.58</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>1.6</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1">
         <v>1</v>
@@ -738,23 +2745,25 @@
       <c r="D20" s="1">
         <v>3</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1">
         <v>4</v>
       </c>
-      <c r="F20" s="1">
+      <c r="H20" s="1">
         <v>5</v>
       </c>
-      <c r="G20" s="1">
+      <c r="I20" s="1">
         <v>6</v>
       </c>
-      <c r="H20" s="1">
+      <c r="J20" s="1">
         <v>7</v>
       </c>
-      <c r="I20" s="1">
+      <c r="K20" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -767,12 +2776,8 @@
       <c r="D21" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
         <v>0</v>
       </c>
@@ -782,8 +2787,14 @@
       <c r="I21" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>7</v>
       </c>
@@ -796,14 +2807,10 @@
       <c r="D22" s="4">
         <v>6</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4">
         <v>6</v>
-      </c>
-      <c r="F22" s="4">
-        <v>11</v>
-      </c>
-      <c r="G22" s="4">
-        <v>11</v>
       </c>
       <c r="H22" s="4">
         <v>11</v>
@@ -811,8 +2818,14 @@
       <c r="I22" s="4">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="4">
+        <v>11</v>
+      </c>
+      <c r="K22" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -825,23 +2838,25 @@
       <c r="D23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="J23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I23" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -851,8 +2866,10 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1">
         <v>9</v>
@@ -863,23 +2880,25 @@
       <c r="D25" s="1">
         <v>11</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1">
         <v>12</v>
       </c>
-      <c r="F25" s="1">
+      <c r="H25" s="1">
         <v>13</v>
       </c>
-      <c r="G25" s="1">
+      <c r="I25" s="1">
         <v>14</v>
       </c>
-      <c r="H25" s="1">
+      <c r="J25" s="1">
         <v>15</v>
       </c>
-      <c r="I25" s="1">
+      <c r="K25" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -892,12 +2911,8 @@
       <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
       <c r="G26" s="3" t="s">
         <v>5</v>
       </c>
@@ -907,8 +2922,14 @@
       <c r="I26" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>7</v>
       </c>
@@ -921,14 +2942,10 @@
       <c r="D27" s="4">
         <v>6</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4">
         <v>6</v>
-      </c>
-      <c r="F27" s="4">
-        <v>11</v>
-      </c>
-      <c r="G27" s="4">
-        <v>11</v>
       </c>
       <c r="H27" s="4">
         <v>11</v>
@@ -936,8 +2953,14 @@
       <c r="I27" s="4">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="4">
+        <v>11</v>
+      </c>
+      <c r="K27" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -950,24 +2973,48 @@
       <c r="D28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G28" s="2" t="s">
+      <c r="H28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="J28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="K28" s="2" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="T7" r:id="rId1" xr:uid="{6073D5B9-973F-4AD5-9FF3-E1F7453687A0}"/>
+    <hyperlink ref="T3" r:id="rId2" xr:uid="{3B360ABD-6B06-4AF7-9ED9-111B14112B1F}"/>
+    <hyperlink ref="T4" r:id="rId3" xr:uid="{311D03A5-1863-456D-9C4E-7B75F8147362}"/>
+    <hyperlink ref="T5" r:id="rId4" xr:uid="{1B83CCB2-7795-40B3-98B5-D5E730D4206B}"/>
+    <hyperlink ref="T6" r:id="rId5" xr:uid="{F50CC0C3-7FA4-4818-8BDE-484D35E104C2}"/>
+    <hyperlink ref="T8" r:id="rId6" xr:uid="{CFC35985-A6A4-49A0-9103-1B373693F1D2}"/>
+    <hyperlink ref="T11" r:id="rId7" xr:uid="{6B0D8177-0ECD-48DC-8425-E122EB83A2C3}"/>
+    <hyperlink ref="T12" r:id="rId8" xr:uid="{15B84114-40B7-42AC-A990-C5A1A2D23FB1}"/>
+    <hyperlink ref="T14" r:id="rId9" xr:uid="{622A3EC3-9300-4092-A082-38B0B38D5617}"/>
+    <hyperlink ref="T15" r:id="rId10" xr:uid="{750F9486-F581-46CC-8B09-8E6FCC9E7428}"/>
+    <hyperlink ref="T16" r:id="rId11" xr:uid="{63FA826C-777B-496D-BD34-BD90598ACEEE}"/>
+    <hyperlink ref="T17" r:id="rId12" xr:uid="{1B66B0A8-6A91-43B9-9CCD-48330BC92F69}"/>
+    <hyperlink ref="T18" r:id="rId13" xr:uid="{3032AF38-8247-4F02-88AC-7E8C6979A033}"/>
+    <hyperlink ref="T9" r:id="rId14" xr:uid="{F22F6BB2-8037-464A-AB43-70CEE7DD78E7}"/>
+    <hyperlink ref="T10" r:id="rId15" xr:uid="{9356E43C-397C-4164-B39A-A4F3C3DA8934}"/>
+    <hyperlink ref="T13" r:id="rId16" xr:uid="{F2E1E623-ECFF-4D05-8642-D1DC034F56E3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>